<commit_message>
updated cases --> making them data driven via excel
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -3,31 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabh Singh\eclipse-workspace\recognition\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416FC126-20FE-45A3-9AC4-987F59EB5981}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{06ED2BDD-70AC-438E-A24C-44D3EB31D771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3D71B169-D99A-4718-9F0C-D37316850886}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,26 +23,34 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>test1</t>
+    <t>Login email</t>
   </si>
   <si>
-    <t>test2</t>
+    <t>password</t>
   </si>
   <si>
-    <t>test3</t>
+    <t>vijay+10@vinsol.com</t>
   </si>
   <si>
-    <t>test4</t>
+    <t>1234567a!</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -78,13 +73,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -400,28 +398,35 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{80C823A5-9A47-4496-9C2E-E5504CD0C18B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding free program case
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -3,7 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0A4F8AF7-1741-4E1C-8DD8-F46FF42D3723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabh Singh\eclipse-workspace\recognition\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE325286-79F0-4F49-9EDA-8DA4E2CFA6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -21,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>email</t>
   </si>
@@ -54,6 +58,12 @@
   </si>
   <si>
     <t>Monthly</t>
+  </si>
+  <si>
+    <t>free prog users</t>
+  </si>
+  <si>
+    <t>rishabh.singh+1@snackmagic.com, rishabh.singh+2@snackmagic.com</t>
   </si>
 </sst>
 </file>
@@ -98,9 +108,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -382,64 +397,73 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.21875" customWidth="1"/>
-    <col min="2" max="2" width="34.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.21875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.77734375" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test case add user, delete user, permission , hashtag
</commit_message>
<xml_diff>
--- a/Data/Book1.xlsx
+++ b/Data/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rishabh Singh\eclipse-workspace\recognition\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE325286-79F0-4F49-9EDA-8DA4E2CFA6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{522F86FA-5189-4DB8-BA57-D19DFC124ED8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>email</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>rishabh.singh+1@snackmagic.com, rishabh.singh+2@snackmagic.com</t>
+  </si>
+  <si>
+    <t>add new users</t>
+  </si>
+  <si>
+    <t>rishabh.singh+3@snackmagic.com</t>
   </si>
 </sst>
 </file>
@@ -397,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -466,9 +472,18 @@
         <v>12</v>
       </c>
     </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B1" r:id="rId1" xr:uid="{83955C66-B869-44C1-BE31-C0D25D43974B}"/>
+    <hyperlink ref="B8" r:id="rId2" xr:uid="{7C3D2A50-9EC4-4E42-BDAA-BDBEF65454D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>